<commit_message>
Update IP - EX 24 - Formatacao condicional padrao (Anexo).xlsx
Exercicio
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 24 - Formatacao condicional padrao (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 24 - Formatacao condicional padrao (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8186A8-5961-4F7D-8FE6-5E1B3D2A0A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1983DC0F-CADF-4907-A948-3F55EADC415A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -218,9 +240,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -588,7 +611,7 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -688,6 +711,9 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Moeda" xfId="4" builtinId="4"/>
@@ -697,8 +723,168 @@
     <cellStyle name="SAPBEXfilterDrill" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Vírgula 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="0.39994506668294322"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1267,7 +1453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -1462,7 +1648,7 @@
   <dimension ref="B1:Q31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,6 +2070,25 @@
   <mergeCells count="1">
     <mergeCell ref="B2:Q6"/>
   </mergeCells>
+  <conditionalFormatting sqref="D10:D18">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="greaterThanOrEqual">
+      <formula>0.7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:D31">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>IF($E$23="reprovado",1,0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>IF($E23="aprovado",1,0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>IF($E23="reprovado",1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1893,14 +2098,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1944,10 +2151,16 @@
       <c r="D4" s="24">
         <v>8</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="25">
+        <f xml:space="preserve"> (C4+D4*2)/3</f>
+        <v>6.333333333333333</v>
+      </c>
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="H4" s="24" t="str" cm="1">
+        <f t="array" ref="H4">_xlfn.IFS(E4&gt;=6,"Aprovado",G4&gt;=5,"Aprovado",G4&lt;5,"Reprovado")</f>
+        <v>Aprovado</v>
+      </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1960,12 +2173,21 @@
       <c r="D5" s="24">
         <v>5</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="25">
+        <f t="shared" ref="E5:E8" si="0" xml:space="preserve"> (C5+D5*2)/3</f>
+        <v>4</v>
+      </c>
       <c r="F5" s="24">
         <v>6</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
+      <c r="G5" s="24">
+        <f xml:space="preserve"> (E5+F5)/2</f>
+        <v>5</v>
+      </c>
+      <c r="H5" s="24" t="str" cm="1">
+        <f t="array" ref="H5">_xlfn.IFS(E5&gt;=6,"Aprovado",G5&gt;=5,"Aprovado",G5&lt;5,"Reprovado")</f>
+        <v>Aprovado</v>
+      </c>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1978,10 +2200,16 @@
       <c r="D6" s="24">
         <v>6</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="H6" s="24" t="str" cm="1">
+        <f t="array" ref="H6">_xlfn.IFS(E6&gt;=6,"Aprovado",G6&gt;=5,"Aprovado",G6&lt;5,"Reprovado")</f>
+        <v>Aprovado</v>
+      </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -1994,10 +2222,16 @@
       <c r="D7" s="24">
         <v>7</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="25">
+        <f t="shared" si="0"/>
+        <v>7.333333333333333</v>
+      </c>
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="H7" s="24" t="str" cm="1">
+        <f t="array" ref="H7">_xlfn.IFS(E7&gt;=6,"Aprovado",G7&gt;=5,"Aprovado",G7&lt;5,"Reprovado")</f>
+        <v>Aprovado</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
@@ -2009,12 +2243,21 @@
       <c r="D8" s="24">
         <v>4</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="25">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
       <c r="F8" s="24">
         <v>4</v>
       </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
+      <c r="G8" s="49">
+        <f t="shared" ref="G6:G8" si="1" xml:space="preserve"> (E8+F8)/2</f>
+        <v>3.666666666666667</v>
+      </c>
+      <c r="H8" s="24" t="str" cm="1">
+        <f t="array" ref="H8">_xlfn.IFS(E8&gt;=6,"Aprovado",G8&gt;=5,"Aprovado",G8&lt;5,"Reprovado")</f>
+        <v>Reprovado</v>
+      </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2085,6 +2328,11 @@
   <mergeCells count="1">
     <mergeCell ref="B15:E18"/>
   </mergeCells>
+  <conditionalFormatting sqref="B4:B8">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>IF(H4="Aprovado",1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>